<commit_message>
Changing Transit data for QAS
</commit_message>
<xml_diff>
--- a/TestData/QAS_RebootTestData.xlsx
+++ b/TestData/QAS_RebootTestData.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">1000102092</t>
   </si>
   <si>
-    <t xml:space="preserve">1000102097</t>
+    <t xml:space="preserve">1000104331</t>
   </si>
   <si>
     <t xml:space="preserve">1000104038</t>
@@ -235,11 +235,11 @@
   </sheetPr>
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.43"/>
@@ -304,7 +304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>19</v>
       </c>

</xml_diff>